<commit_message>
Fixed relative path errors
</commit_message>
<xml_diff>
--- a/Predictions/Week 3/Week 3.xlsx
+++ b/Predictions/Week 3/Week 3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg_yonan\Desktop\Tools\Programs\NFL\2025 Season\Predictions\Week 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7537FFB-0295-4EDA-90C8-DABF64895B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63DEA79-CCE6-4B0F-9BAB-F3D0E9B8EB8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -157,7 +157,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,6 +204,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFBFBFBF"/>
         <bgColor rgb="FFBFBFBF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -254,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -279,6 +285,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,19 +657,19 @@
       <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="10" t="s">
         <v>9</v>
       </c>
     </row>
@@ -671,19 +680,19 @@
       <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="10" t="s">
         <v>11</v>
       </c>
     </row>
@@ -707,7 +716,7 @@
         <v>13</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -717,19 +726,19 @@
       <c r="B6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="10" t="s">
         <v>15</v>
       </c>
     </row>
@@ -789,13 +798,13 @@
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="10" t="s">
         <v>22</v>
       </c>
       <c r="G9" s="8" t="s">
@@ -809,7 +818,7 @@
       <c r="B10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="10" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="8" t="s">
@@ -832,16 +841,16 @@
       <c r="B11" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="10" t="s">
         <v>25</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="10" t="s">
         <v>25</v>
       </c>
       <c r="G11" s="8" t="s">
@@ -907,13 +916,13 @@
       <c r="D14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="10" t="s">
         <v>31</v>
       </c>
     </row>
@@ -924,16 +933,16 @@
       <c r="B15" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="10" t="s">
         <v>33</v>
       </c>
       <c r="G15" s="8" t="s">
@@ -950,7 +959,7 @@
       <c r="C16" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="10" t="s">
         <v>36</v>
       </c>
       <c r="E16" s="8" t="s">
@@ -970,20 +979,37 @@
       <c r="B17" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="11" t="s">
         <v>38</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G17" s="11" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="12">
+        <v>0.5625</v>
+      </c>
+      <c r="D18" s="12">
+        <v>0.5625</v>
+      </c>
+      <c r="E18" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="F18" s="12">
+        <v>0.5625</v>
+      </c>
+      <c r="G18" s="12">
+        <v>0.6875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>